<commit_message>
Update AZ for REST
</commit_message>
<xml_diff>
--- a/CSC3510 S2021/Lectures/NodeJSExpress.xlsx
+++ b/CSC3510 S2021/Lectures/NodeJSExpress.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\dlash\github\CSC3510\S2021\Lectures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlash\Documents\GitHub\CSC3510\CSC3510 S2021\Lectures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2268E6AC-5423-439B-A549-1C9BFA28B2D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="7" activeTab="7" xr2:uid="{206C531E-3F85-4014-8729-D7C561154CFF}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" firstSheet="10" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Express" sheetId="1" r:id="rId1"/>
@@ -71,7 +70,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -293,16 +292,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>360045</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>379095</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>173836</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>178624</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>192886</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>102424</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -325,8 +324,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8894445" y="5657850"/>
-          <a:ext cx="11396191" cy="3569524"/>
+          <a:off x="7084695" y="6257925"/>
+          <a:ext cx="11396191" cy="3750499"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1103,6 +1102,216 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1660647" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8677275" y="1181100"/>
+          <a:ext cx="1660647" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>npm install --save express</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="7302577" cy="1125693"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8886825" y="1781175"/>
+          <a:ext cx="7302577" cy="1125693"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Had to add the following to package-lock.json</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>"os": </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>[</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>"darwin",</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  "win32"</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>,</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>https://stackoverflow.com/questions/56103865/how-to-fix-unsupported-platform-for-fsevents1-2-9-wanted-osdarwin-arch</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2437,6 +2646,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1400" b="0">
               <a:solidFill>
@@ -2532,6 +2753,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1400" b="0">
               <a:solidFill>
@@ -2893,6 +3126,13 @@
             </a:rPr>
             <a:t>var con = mysql.createConnection({</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -2911,6 +3151,13 @@
             </a:rPr>
             <a:t>  host: "localhost",</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -2953,6 +3200,13 @@
             </a:rPr>
             <a:t>",</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -2995,6 +3249,13 @@
             </a:rPr>
             <a:t>",</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3013,6 +3274,13 @@
             </a:rPr>
             <a:t>  database: "mydb"</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3031,12 +3299,26 @@
             </a:rPr>
             <a:t>});</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
           </a:br>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3055,6 +3337,13 @@
             </a:rPr>
             <a:t>con.connect(function(err) {</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3073,6 +3362,13 @@
             </a:rPr>
             <a:t>  if (err) throw err;</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3091,6 +3387,13 @@
             </a:rPr>
             <a:t>  console.log("Connected!");</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3132,6 +3435,13 @@
             </a:rPr>
             <a:t>  con.query(sql, function (err, result) {</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3150,6 +3460,13 @@
             </a:rPr>
             <a:t>    if (err) throw err;</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3168,6 +3485,13 @@
             </a:rPr>
             <a:t>    console.log("1 record inserted");</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3185,6 +3509,13 @@
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
             <a:t>  });</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
           </a:r>
           <a:br>
             <a:rPr lang="en-US">
@@ -3279,12 +3610,26 @@
             </a:rPr>
             <a:t>var mysql = require('mysql');</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
           </a:br>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3303,6 +3648,13 @@
             </a:rPr>
             <a:t>var con = mysql.createConnection({</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3321,6 +3673,13 @@
             </a:rPr>
             <a:t>  host: "localhost",</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3339,6 +3698,13 @@
             </a:rPr>
             <a:t>  user: "yourusername",</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3357,6 +3723,13 @@
             </a:rPr>
             <a:t>  password: "yourpassword",</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3375,6 +3748,13 @@
             </a:rPr>
             <a:t>  database: "mydb"</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3393,12 +3773,26 @@
             </a:rPr>
             <a:t>});</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
           </a:br>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3417,6 +3811,13 @@
             </a:rPr>
             <a:t>con.connect(function(err) {</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3435,6 +3836,13 @@
             </a:rPr>
             <a:t>  if (err) throw err;</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3476,6 +3884,13 @@
             </a:rPr>
             <a:t>  con.query(sql, function (err, result) {</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3494,6 +3909,13 @@
             </a:rPr>
             <a:t>    if (err) throw err;</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3512,6 +3934,13 @@
             </a:rPr>
             <a:t>    console.log("Number of records deleted: " + result.affectedRows);</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
               <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
@@ -3529,6 +3958,13 @@
               <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
             </a:rPr>
             <a:t>  });</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1">
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
           </a:r>
           <a:br>
             <a:rPr lang="en-US" b="1">
@@ -3864,6 +4300,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1400" b="0">
               <a:solidFill>
@@ -3959,6 +4407,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1400" b="0">
               <a:solidFill>
@@ -4054,6 +4514,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1400" b="0">
               <a:solidFill>
@@ -4107,6 +4579,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1400" b="0">
               <a:solidFill>
@@ -4216,6 +4700,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1400" b="0">
               <a:solidFill>
@@ -7028,6 +7524,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1100" b="0">
               <a:solidFill>
@@ -7081,6 +7589,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1100" b="0">
               <a:solidFill>
@@ -7120,6 +7640,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1100" b="0">
               <a:solidFill>
@@ -7201,6 +7733,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1100" b="0">
               <a:solidFill>
@@ -10318,6 +10862,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1100" b="0">
               <a:solidFill>
@@ -10413,6 +10969,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Courier New" panose="02070309020205020404" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1100" b="0">
               <a:solidFill>
@@ -10540,6 +11108,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1200" b="0">
               <a:solidFill>
@@ -10565,6 +11145,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1200" b="0">
               <a:solidFill>
@@ -10604,6 +11196,18 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
           <a:br>
             <a:rPr lang="en-US" sz="1200" b="0">
               <a:solidFill>
@@ -15888,21 +16492,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ACE312-05FC-4BE0-A2B7-EDF92541167E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="Q26:Q27"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="26" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q26" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="17:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q27" t="s">
         <v>0</v>
       </c>
@@ -15914,16 +16518,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B237AEAE-47ED-49A6-98AE-4A9F4C887404}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="24" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K24" t="s">
         <v>3</v>
       </c>
@@ -15935,16 +16539,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EC39D8A-8876-4274-848B-CFEFD35147FC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="8.21875" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15953,16 +16557,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745CF115-4FB9-488A-A0D9-CC1B9B661C7B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="T2"/>
   <sheetViews>
     <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="20:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="20:20" x14ac:dyDescent="0.25">
       <c r="T2" t="s">
         <v>6</v>
       </c>
@@ -15974,14 +16578,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE099076-2A6D-4BB3-B974-BB005C8DC6C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15989,14 +16593,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797E635E-FBAB-41FB-851F-DBAACB2C88FF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16004,14 +16608,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90C6012-6767-4167-BC5B-41233A2095CB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="Q44" sqref="P44:Q44"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16019,14 +16623,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666668EF-6D9B-4493-A372-B35A7159CC06}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16035,16 +16639,16 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38D09776-6969-4A9E-B061-68F3903659FF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="X32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="32" spans="24:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="24:24" x14ac:dyDescent="0.25">
       <c r="X32" t="s">
         <v>2</v>
       </c>
@@ -16056,21 +16660,21 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A01665-2497-4CD6-AC3C-D587772BAC69}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A33"/>
   <sheetViews>
     <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -16082,14 +16686,14 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D37E4D-35A3-44E2-8587-839D43D04A61}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16097,21 +16701,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6276FEDA-AAE9-471A-B5CD-9CABE42C425F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D19:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="1"/>
     </row>
   </sheetData>
@@ -16121,14 +16725,14 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6556BC3-BF8E-4ABB-9152-22B78ACC0F9E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16136,14 +16740,14 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F20DCC2-5F1F-485E-8FCC-95FE2CAE343F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16151,16 +16755,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7236FF81-9CE6-4FE5-9044-9D1579FF8613}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G30" s="1"/>
     </row>
   </sheetData>
@@ -16170,16 +16774,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F66707F-FED2-4A97-9CAE-0BB236C3A9C7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H23"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="A4" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
         <v>2</v>
       </c>
@@ -16191,14 +16795,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28886FC9-EEBD-4E75-BEC9-EAA135E4926A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="A7" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16206,14 +16810,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7876C246-E13D-4DFD-8DEE-5B39CF724F65}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="B79" workbookViewId="0">
       <selection activeCell="F105" sqref="F105:F106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16221,14 +16825,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D346582-6303-4C12-8F1C-E75852D7467E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16236,16 +16840,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26EA5BD-6CF0-4EDE-ADFE-D6E8AF286E49}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="H71" sqref="H71"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="Q76" sqref="Q76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="75" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H75" t="s">
         <v>5</v>
       </c>
@@ -16257,21 +16861,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C59B3FE-3277-402F-996B-AC8B0FAAA9DA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B154:D176"/>
   <sheetViews>
     <sheetView topLeftCell="B154" workbookViewId="0">
       <selection activeCell="V153" sqref="V153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D154" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
         <v>1</v>
       </c>

</xml_diff>